<commit_message>
ElecTRADE: adding price-setting plot, cleaning the non-fossil building
</commit_message>
<xml_diff>
--- a/data/raw/Calibration_Capacity_nonfossilfuel_mannualcollection-2025.xlsx
+++ b/data/raw/Calibration_Capacity_nonfossilfuel_mannualcollection-2025.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhang/Resource/China-ElecTrade-APP/China-Daily-ElecTRADE/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhang/Resource/China-ElecTrade-APP/Pypsa-Draworld-ElecTRADE/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24C2982B-040A-884B-B4FB-E5866AA92DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8170F23-2807-584D-A0B8-B5182083D398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22480" yWindow="1300" windowWidth="38860" windowHeight="24160" activeTab="1" xr2:uid="{25A1E0AA-52D8-3B4D-AF14-8AC2B10B3F77}"/>
+    <workbookView xWindow="12340" yWindow="1300" windowWidth="38860" windowHeight="24160" xr2:uid="{25A1E0AA-52D8-3B4D-AF14-8AC2B10B3F77}"/>
   </bookViews>
   <sheets>
     <sheet name="cap0_2025" sheetId="1" r:id="rId1"/>
-    <sheet name="network" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId2"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -164,18 +163,6 @@
     <t>Simulation Year</t>
   </si>
   <si>
-    <t>Hebei_HEBEI_NORTH</t>
-  </si>
-  <si>
-    <t>Hebei_HEBEI_SOUTH</t>
-  </si>
-  <si>
-    <t>Inner Mongolia_NM_EAST</t>
-  </si>
-  <si>
-    <t>Inner Mongolia_NM_WEST</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
@@ -210,6 +197,18 @@
   </si>
   <si>
     <t>Source: 抽水蓄能：https://www.sohu.com/a/798091551_120018660； https://www.escn.com.cn/news/show-2125311.html</t>
+  </si>
+  <si>
+    <t>HEBEI_NORTH</t>
+  </si>
+  <si>
+    <t>HEBEI_SOUTH</t>
+  </si>
+  <si>
+    <t>NM_EAST</t>
+  </si>
+  <si>
+    <t>NM_WEST</t>
   </si>
 </sst>
 </file>
@@ -513,8 +512,8 @@
       <sheetName val="template (2)"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
       <sheetData sheetId="2">
         <row r="3">
           <cell r="H3">
@@ -598,7 +597,7 @@
         </row>
         <row r="22">
           <cell r="H22">
-            <v>66.847000000000008</v>
+            <v>66.846999999999994</v>
           </cell>
         </row>
         <row r="23">
@@ -643,7 +642,7 @@
         </row>
         <row r="33">
           <cell r="H33">
-            <v>27.090000000000003</v>
+            <v>27.09</v>
           </cell>
         </row>
         <row r="35">
@@ -682,21 +681,21 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1004,11 +1003,11 @@
   </sheetPr>
   <dimension ref="A1:W998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1062,7 +1061,7 @@
         <v>5</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
@@ -1071,19 +1070,19 @@
         <v>8</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>9</v>
@@ -1098,10 +1097,10 @@
         <v>11</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
@@ -1119,7 +1118,7 @@
       </c>
       <c r="D3" s="12">
         <f t="shared" ref="D3:D8" si="0">SUM(E3:R3)</f>
-        <v>13.5</v>
+        <v>15.8</v>
       </c>
       <c r="E3" s="6">
         <v>0</v>
@@ -1136,11 +1135,15 @@
       <c r="I3" s="6">
         <v>1</v>
       </c>
-      <c r="J3" s="6"/>
+      <c r="J3" s="6">
+        <v>0.3</v>
+      </c>
       <c r="K3" s="6">
         <v>0</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="6">
+        <v>2</v>
+      </c>
       <c r="M3" s="6">
         <v>0</v>
       </c>
@@ -1175,7 +1178,7 @@
       </c>
       <c r="D4" s="12">
         <f t="shared" si="0"/>
-        <v>20.7</v>
+        <v>32.700000000000003</v>
       </c>
       <c r="E4" s="6">
         <v>16</v>
@@ -1192,11 +1195,15 @@
       <c r="I4" s="6">
         <v>0</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="6">
+        <v>2</v>
+      </c>
       <c r="K4" s="6">
         <v>0</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="6">
+        <v>10</v>
+      </c>
       <c r="M4" s="6">
         <v>0</v>
       </c>
@@ -1223,7 +1230,7 @@
         <v>2025</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C5" s="11">
         <f>[1]load!H6</f>
@@ -1287,7 +1294,7 @@
         <v>2025</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C6" s="11">
         <f>[1]load!H5</f>
@@ -1357,7 +1364,7 @@
       </c>
       <c r="D7" s="12">
         <f t="shared" si="0"/>
-        <v>114.17</v>
+        <v>164.17</v>
       </c>
       <c r="E7" s="6">
         <f>80.11-SUM(F7:G7)</f>
@@ -1381,7 +1388,9 @@
       <c r="K7" s="6">
         <v>0</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="6">
+        <v>50</v>
+      </c>
       <c r="M7" s="6">
         <v>2.7</v>
       </c>
@@ -1491,7 +1500,7 @@
         <v>2025</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="C10" s="11">
         <f>[1]load!H10</f>
@@ -1562,7 +1571,7 @@
       </c>
       <c r="D11" s="12">
         <f>SUM(E11:R11)</f>
-        <v>52.379999999999995</v>
+        <v>87.13</v>
       </c>
       <c r="E11" s="6">
         <v>32.799999999999997</v>
@@ -1579,11 +1588,15 @@
       <c r="I11" s="6">
         <v>3</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="J11" s="6">
+        <v>20</v>
+      </c>
       <c r="K11" s="6">
-        <v>1.5</v>
-      </c>
-      <c r="L11" s="6"/>
+        <v>1.25</v>
+      </c>
+      <c r="L11" s="6">
+        <v>15</v>
+      </c>
       <c r="M11" s="6">
         <v>2.8</v>
       </c>
@@ -1618,7 +1631,7 @@
       </c>
       <c r="D12" s="12">
         <f>SUM(E12:R12)</f>
-        <v>27.949999999999996</v>
+        <v>44.949999999999996</v>
       </c>
       <c r="E12" s="6">
         <v>16.7</v>
@@ -1635,11 +1648,15 @@
       <c r="I12" s="6">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J12" s="6"/>
+      <c r="J12" s="6">
+        <v>10</v>
+      </c>
       <c r="K12" s="6">
         <v>0</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="6">
+        <v>7</v>
+      </c>
       <c r="M12" s="6">
         <v>2.25</v>
       </c>
@@ -1674,7 +1691,7 @@
       </c>
       <c r="D13" s="12">
         <f>SUM(E13:R13)</f>
-        <v>29.5</v>
+        <v>57.5</v>
       </c>
       <c r="E13" s="6">
         <v>21.8</v>
@@ -1691,11 +1708,15 @@
       <c r="I13" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J13" s="6"/>
+      <c r="J13" s="6">
+        <v>19</v>
+      </c>
       <c r="K13" s="6">
         <v>0</v>
       </c>
-      <c r="L13" s="14"/>
+      <c r="L13" s="14">
+        <v>9</v>
+      </c>
       <c r="M13" s="6">
         <v>1.2</v>
       </c>
@@ -2077,7 +2098,7 @@
       </c>
       <c r="D21" s="12">
         <f>SUM(E21:R21)</f>
-        <v>35.400000000000006</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="E21" s="6">
         <v>22.1</v>
@@ -2094,11 +2115,15 @@
       <c r="I21" s="6">
         <v>6.6</v>
       </c>
-      <c r="J21" s="6"/>
+      <c r="J21" s="6">
+        <v>7</v>
+      </c>
       <c r="K21" s="6">
         <v>0</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="6">
+        <v>30</v>
+      </c>
       <c r="M21" s="6">
         <v>1.2</v>
       </c>
@@ -2129,7 +2154,7 @@
       </c>
       <c r="C22" s="11">
         <f>[1]load!H22</f>
-        <v>66.847000000000008</v>
+        <v>66.846999999999994</v>
       </c>
       <c r="D22" s="12">
         <f>SUM(E22:R22)</f>
@@ -2194,7 +2219,7 @@
       </c>
       <c r="D23" s="12">
         <f>SUM(E23:R23)</f>
-        <v>77.22</v>
+        <v>123.72</v>
       </c>
       <c r="E23" s="6">
         <v>32.799999999999997</v>
@@ -2211,11 +2236,15 @@
       <c r="I23" s="6">
         <v>38.119999999999997</v>
       </c>
-      <c r="J23" s="6"/>
+      <c r="J23" s="6">
+        <v>1.5</v>
+      </c>
       <c r="K23" s="6">
         <v>0</v>
       </c>
-      <c r="L23" s="6"/>
+      <c r="L23" s="6">
+        <v>45</v>
+      </c>
       <c r="M23" s="6">
         <v>0</v>
       </c>
@@ -2250,7 +2279,7 @@
       </c>
       <c r="D24" s="12">
         <f>SUM(E24:R24)</f>
-        <v>47.19</v>
+        <v>84.19</v>
       </c>
       <c r="E24" s="6">
         <v>23.46</v>
@@ -2267,11 +2296,15 @@
       <c r="I24" s="6">
         <v>16.37</v>
       </c>
-      <c r="J24" s="6"/>
+      <c r="J24" s="6">
+        <v>12</v>
+      </c>
       <c r="K24" s="6">
         <v>0</v>
       </c>
-      <c r="L24" s="6"/>
+      <c r="L24" s="6">
+        <v>25</v>
+      </c>
       <c r="M24" s="6">
         <v>1.4</v>
       </c>
@@ -2328,7 +2361,7 @@
       </c>
       <c r="D26" s="12">
         <f>SUM(E26:R26)</f>
-        <v>28.8</v>
+        <v>36.800000000000004</v>
       </c>
       <c r="E26" s="6">
         <v>15</v>
@@ -2345,11 +2378,15 @@
       <c r="I26" s="6">
         <v>7.8</v>
       </c>
-      <c r="J26" s="6"/>
+      <c r="J26" s="6">
+        <v>3</v>
+      </c>
       <c r="K26" s="6">
         <v>0</v>
       </c>
-      <c r="L26" s="6"/>
+      <c r="L26" s="6">
+        <v>5</v>
+      </c>
       <c r="M26" s="6">
         <v>1.2</v>
       </c>
@@ -2384,7 +2421,7 @@
       </c>
       <c r="D27" s="12">
         <f>SUM(E27:R27)</f>
-        <v>121.80000000000001</v>
+        <v>146.80000000000001</v>
       </c>
       <c r="E27" s="6">
         <v>13.6</v>
@@ -2401,11 +2438,15 @@
       <c r="I27" s="6">
         <v>97.7</v>
       </c>
-      <c r="J27" s="6"/>
+      <c r="J27" s="6">
+        <v>9</v>
+      </c>
       <c r="K27" s="6">
         <v>0</v>
       </c>
-      <c r="L27" s="6"/>
+      <c r="L27" s="6">
+        <v>16</v>
+      </c>
       <c r="M27" s="6">
         <v>0</v>
       </c>
@@ -2515,7 +2556,7 @@
         <v>2025</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C30" s="11">
         <f>[1]load!H30</f>
@@ -2523,7 +2564,7 @@
       </c>
       <c r="D30" s="12">
         <f>SUM(E30:R30)</f>
-        <v>50.97</v>
+        <v>105.97</v>
       </c>
       <c r="E30" s="6">
         <v>21.1</v>
@@ -2540,11 +2581,15 @@
       <c r="I30" s="6">
         <v>19.04</v>
       </c>
-      <c r="J30" s="6"/>
+      <c r="J30" s="6">
+        <v>25</v>
+      </c>
       <c r="K30" s="6">
         <v>0</v>
       </c>
-      <c r="L30" s="6"/>
+      <c r="L30" s="6">
+        <v>30</v>
+      </c>
       <c r="M30" s="6">
         <v>0</v>
       </c>
@@ -2579,7 +2624,7 @@
       </c>
       <c r="D31" s="12">
         <f>SUM(E31:R31)</f>
-        <v>9.7000000000000011</v>
+        <v>21.700000000000003</v>
       </c>
       <c r="E31" s="6">
         <v>4.9000000000000004</v>
@@ -2596,11 +2641,15 @@
       <c r="I31" s="6">
         <v>1.5</v>
       </c>
-      <c r="J31" s="6"/>
+      <c r="J31" s="6">
+        <v>2</v>
+      </c>
       <c r="K31" s="6">
         <v>0</v>
       </c>
-      <c r="L31" s="6"/>
+      <c r="L31" s="6">
+        <v>10</v>
+      </c>
       <c r="M31" s="6">
         <v>0</v>
       </c>
@@ -2635,7 +2684,7 @@
       </c>
       <c r="D32" s="12">
         <f>SUM(E32:R32)</f>
-        <v>61.58</v>
+        <v>101.58</v>
       </c>
       <c r="E32" s="6">
         <v>32</v>
@@ -2652,11 +2701,15 @@
       <c r="I32" s="6">
         <v>22.98</v>
       </c>
-      <c r="J32" s="6"/>
+      <c r="J32" s="6">
+        <v>10</v>
+      </c>
       <c r="K32" s="6">
         <v>0</v>
       </c>
-      <c r="L32" s="6"/>
+      <c r="L32" s="6">
+        <v>30</v>
+      </c>
       <c r="M32" s="6">
         <v>0</v>
       </c>
@@ -2687,11 +2740,11 @@
       </c>
       <c r="C33" s="11">
         <f>[1]load!H33</f>
-        <v>27.090000000000003</v>
+        <v>27.09</v>
       </c>
       <c r="D33" s="12">
         <f>SUM(E33:R33)</f>
-        <v>105.69999999999999</v>
+        <v>167.7</v>
       </c>
       <c r="E33" s="6">
         <v>13.6</v>
@@ -2708,11 +2761,15 @@
       <c r="I33" s="6">
         <v>83.6</v>
       </c>
-      <c r="J33" s="6"/>
+      <c r="J33" s="6">
+        <v>12</v>
+      </c>
       <c r="K33" s="6">
         <v>0</v>
       </c>
-      <c r="L33" s="6"/>
+      <c r="L33" s="6">
+        <v>50</v>
+      </c>
       <c r="M33" s="6">
         <v>0</v>
       </c>
@@ -2769,7 +2826,7 @@
       </c>
       <c r="D35" s="12">
         <f>SUM(E35:R35)</f>
-        <v>64.06</v>
+        <v>116.06</v>
       </c>
       <c r="E35" s="6">
         <f>56.76-SUM(F35:G35)</f>
@@ -2787,11 +2844,15 @@
       <c r="I35" s="6">
         <v>3.9</v>
       </c>
-      <c r="J35" s="6"/>
+      <c r="J35" s="6">
+        <v>12</v>
+      </c>
       <c r="K35" s="6">
         <v>0</v>
       </c>
-      <c r="L35" s="6"/>
+      <c r="L35" s="6">
+        <v>40</v>
+      </c>
       <c r="M35" s="6">
         <v>1.4</v>
       </c>
@@ -2826,7 +2887,7 @@
       </c>
       <c r="D36" s="12">
         <f>SUM(E36:R36)</f>
-        <v>69.849999999999994</v>
+        <v>109.85</v>
       </c>
       <c r="E36" s="6">
         <v>21.9</v>
@@ -2849,7 +2910,9 @@
       <c r="K36" s="6">
         <v>0</v>
       </c>
-      <c r="L36" s="6"/>
+      <c r="L36" s="6">
+        <v>40</v>
+      </c>
       <c r="M36" s="6">
         <v>0</v>
       </c>
@@ -2884,7 +2947,7 @@
       </c>
       <c r="D37" s="12">
         <f>SUM(E37:R37)</f>
-        <v>22.299999999999997</v>
+        <v>75.3</v>
       </c>
       <c r="E37" s="6">
         <v>3.7</v>
@@ -2901,11 +2964,15 @@
       <c r="I37" s="6">
         <v>16.399999999999999</v>
       </c>
-      <c r="J37" s="6"/>
+      <c r="J37" s="6">
+        <v>13</v>
+      </c>
       <c r="K37" s="6">
         <v>0</v>
       </c>
-      <c r="L37" s="6"/>
+      <c r="L37" s="6">
+        <v>40</v>
+      </c>
       <c r="M37" s="6">
         <v>0</v>
       </c>
@@ -2940,7 +3007,7 @@
       </c>
       <c r="D38" s="12">
         <f>SUM(E38:R38)</f>
-        <v>39.130000000000003</v>
+        <v>92.13</v>
       </c>
       <c r="E38" s="6">
         <v>31.6</v>
@@ -2957,11 +3024,15 @@
       <c r="I38" s="6">
         <v>0.4</v>
       </c>
-      <c r="J38" s="6"/>
+      <c r="J38" s="6">
+        <v>18</v>
+      </c>
       <c r="K38" s="6">
         <v>0</v>
       </c>
-      <c r="L38" s="6"/>
+      <c r="L38" s="6">
+        <v>35</v>
+      </c>
       <c r="M38" s="6">
         <v>0</v>
       </c>
@@ -3071,7 +3142,7 @@
         <v>2025</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C41" s="11">
         <f>[1]load!H41</f>
@@ -3176,7 +3247,7 @@
       </c>
       <c r="D43" s="12">
         <f>SUM(E43:R43)</f>
-        <v>3.6</v>
+        <v>8.6</v>
       </c>
       <c r="E43" s="6">
         <v>0.4</v>
@@ -3199,7 +3270,9 @@
       <c r="K43" s="6">
         <v>0</v>
       </c>
-      <c r="L43" s="6"/>
+      <c r="L43" s="6">
+        <v>5</v>
+      </c>
       <c r="M43" s="6">
         <v>0</v>
       </c>
@@ -3248,7 +3321,7 @@
         <v>2025</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="6">
@@ -3277,7 +3350,7 @@
         <v>2025</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="19">
@@ -3325,7 +3398,7 @@
     </row>
     <row r="48" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
@@ -27112,16 +27185,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28416C75-5C33-F543-A316-57BADBB06F03}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>